<commit_message>
Updates data in project list template
</commit_message>
<xml_diff>
--- a/project_input_template/project_list.xlsx
+++ b/project_input_template/project_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akey/PublicLandBOSSE_Data/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aeberle/Documents/GitHub/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE8645F-C62E-D443-B334-9FBE7BCDF1AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0C19A2-9323-7D47-98A0-D293C41858CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22460" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="19940" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -521,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Y3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,7 +759,7 @@
         <v>8</v>
       </c>
       <c r="AD2">
-        <v>12.2</v>
+        <v>11</v>
       </c>
       <c r="AE2">
         <v>10</v>

</xml_diff>

<commit_message>
Integrated Distributed and Hybrid Integration changes. Fixed a few bugs that I found.
</commit_message>
<xml_diff>
--- a/project_input_template/project_list.xlsx
+++ b/project_input_template/project_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akey/PublicProjects/WISDEM-LandBOSSE/LandBOSSE/project_input_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/banderso2/Documents/PublicLandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A0CBCB-894B-A040-A3D9-BB816441F490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F30DFB-9941-FE4E-AF46-C6635148FE3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="440" windowWidth="36760" windowHeight="27340" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Project list" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Project ID</t>
   </si>
@@ -61,6 +69,9 @@
     <t>Foundation depth m</t>
   </si>
   <si>
+    <t>foundation_validation_ge15</t>
+  </si>
+  <si>
     <t>Rated Thrust (N)</t>
   </si>
   <si>
@@ -79,27 +90,27 @@
     <t>Combined Homerun Trench Length to Substation (km)</t>
   </si>
   <si>
+    <t>50-year Gust Velocity (m/s)</t>
+  </si>
+  <si>
     <t>Total project construction time (months)</t>
   </si>
   <si>
-    <t>50-year Gust Velocity (m/s)</t>
-  </si>
-  <si>
     <t>Non-Erection Wind Delay Critical Height (m)</t>
   </si>
   <si>
     <t>Non-Erection Wind Delay Critical Speed (m/s)</t>
   </si>
   <si>
-    <t>Distance to interconnect (miles)</t>
-  </si>
-  <si>
     <t>Interconnect Voltage (kV)</t>
   </si>
   <si>
     <t>New Switchyard (y/n)</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>Road length adder (m)</t>
   </si>
   <si>
@@ -109,12 +120,6 @@
     <t>Percent of roads that will be constructed</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>project_1</t>
-  </si>
-  <si>
     <t>Road width (ft)</t>
   </si>
   <si>
@@ -136,6 +141,9 @@
     <t>Allow same flag</t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
     <t>Markup contingency</t>
   </si>
   <si>
@@ -151,20 +159,50 @@
     <t>Markup profit margin</t>
   </si>
   <si>
-    <t>n</t>
+    <t>Project data file</t>
   </si>
   <si>
     <t>Crane breakdown fraction</t>
   </si>
   <si>
     <t>Labor cost multiplier</t>
+  </si>
+  <si>
+    <t>Override total management cost for distributed (0 does not override)</t>
+  </si>
+  <si>
+    <t>Calculate road cost for distributed wind? (y/n)</t>
+  </si>
+  <si>
+    <t>Site prep area for Distributed wind (m2)</t>
+  </si>
+  <si>
+    <t>private_foundation_validation_ge15</t>
+  </si>
+  <si>
+    <t>public_foundation_validation_ge15</t>
+  </si>
+  <si>
+    <t>project_data_defaults</t>
+  </si>
+  <si>
+    <t>Collection mode</t>
+  </si>
+  <si>
+    <t>Distance to interconnect [mi]</t>
+  </si>
+  <si>
+    <t>manual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +213,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,18 +242,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -520,297 +575,482 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
-  <dimension ref="A1:AO2"/>
+  <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1:AN1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU11" sqref="AU11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="53.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="38" width="10.83203125" style="1"/>
-    <col min="39" max="39" width="25.6640625" style="1" customWidth="1"/>
-    <col min="40" max="40" width="26.83203125" style="1" customWidth="1"/>
-    <col min="41" max="41" width="20" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
+    <col min="18" max="18" width="27.33203125" customWidth="1"/>
+    <col min="19" max="19" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="46" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.5" customWidth="1"/>
+    <col min="22" max="22" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20" customWidth="1"/>
+    <col min="27" max="27" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.33203125" customWidth="1"/>
+    <col min="30" max="30" width="25.5" customWidth="1"/>
+    <col min="31" max="31" width="23" customWidth="1"/>
+    <col min="32" max="32" width="27.5" customWidth="1"/>
+    <col min="33" max="33" width="22.33203125" customWidth="1"/>
+    <col min="34" max="34" width="24.83203125" customWidth="1"/>
+    <col min="35" max="35" width="26.6640625" customWidth="1"/>
+    <col min="36" max="36" width="32" customWidth="1"/>
+    <col min="37" max="37" width="27.33203125" customWidth="1"/>
+    <col min="38" max="38" width="22.6640625" customWidth="1"/>
+    <col min="39" max="39" width="34" customWidth="1"/>
+    <col min="40" max="40" width="24.83203125" customWidth="1"/>
+    <col min="41" max="41" width="24.5" customWidth="1"/>
+    <col min="42" max="42" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>80</v>
+      </c>
+      <c r="F2" s="1">
+        <v>77</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2.36</v>
+      </c>
+      <c r="O2" s="2">
+        <v>589000</v>
+      </c>
+      <c r="P2" s="1">
+        <v>191521</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>59.5</v>
+      </c>
+      <c r="R2" s="1">
+        <v>60</v>
+      </c>
+      <c r="S2" s="1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="T2" s="1">
+        <v>50</v>
+      </c>
+      <c r="U2" s="1">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1">
+        <v>15</v>
+      </c>
+      <c r="W2" s="4">
+        <v>10</v>
+      </c>
+      <c r="X2" s="4">
+        <v>130</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>5000</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>20</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="4">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="AH2" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="AK2" s="4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="AN2" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="AO2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS2" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3">
+        <v>80</v>
+      </c>
+      <c r="F3">
+        <v>77</v>
+      </c>
+      <c r="G3">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>0.8</v>
+      </c>
+      <c r="K3">
+        <v>1.5</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>0.2</v>
+      </c>
+      <c r="N3">
+        <v>2.36</v>
+      </c>
+      <c r="O3" s="3">
+        <v>589000</v>
+      </c>
+      <c r="P3">
+        <v>191521</v>
+      </c>
+      <c r="Q3">
+        <v>59.5</v>
+      </c>
+      <c r="R3">
+        <v>60</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>50</v>
+      </c>
+      <c r="U3">
+        <v>10</v>
+      </c>
+      <c r="V3">
+        <v>15</v>
+      </c>
+      <c r="W3" s="10">
+        <v>10</v>
+      </c>
+      <c r="X3" s="10">
+        <v>130</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="10">
+        <v>5000</v>
+      </c>
+      <c r="AA3" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="AC3" s="10">
+        <v>20</v>
+      </c>
+      <c r="AD3" s="10">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AE3" s="10">
+        <v>12.2</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>10</v>
+      </c>
+      <c r="AG3" s="10">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ3" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AK3" s="10">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AL3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AN3" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AO3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>43</v>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>1.5</v>
-      </c>
-      <c r="D2">
-        <v>80</v>
-      </c>
-      <c r="E2">
-        <v>77</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>67</v>
-      </c>
-      <c r="I2">
-        <v>0.7</v>
-      </c>
-      <c r="J2">
-        <v>1.5</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>0.2</v>
-      </c>
-      <c r="M2">
-        <v>2.36</v>
-      </c>
-      <c r="N2" s="3">
-        <v>589000</v>
-      </c>
-      <c r="O2">
-        <v>191521</v>
-      </c>
-      <c r="P2">
-        <v>59.5</v>
-      </c>
-      <c r="Q2">
-        <v>60</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>50</v>
-      </c>
-      <c r="T2">
-        <v>10</v>
-      </c>
-      <c r="U2">
-        <v>15</v>
-      </c>
-      <c r="V2">
-        <v>5</v>
-      </c>
-      <c r="W2">
-        <v>130</v>
-      </c>
-      <c r="X2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2">
-        <v>5000</v>
-      </c>
-      <c r="Z2">
-        <v>0.6</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>0.33</v>
-      </c>
-      <c r="AB2">
-        <v>20</v>
-      </c>
-      <c r="AC2">
-        <v>8</v>
-      </c>
-      <c r="AD2">
-        <v>11</v>
-      </c>
-      <c r="AE2">
-        <v>10</v>
-      </c>
-      <c r="AF2">
-        <v>2</v>
-      </c>
-      <c r="AG2">
-        <v>1.4</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI2">
-        <v>0.03</v>
-      </c>
-      <c r="AJ2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <v>0.05</v>
-      </c>
-      <c r="AM2">
-        <v>0.05</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="2">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="O4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -819,7 +1059,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E92228-1010-354F-B5D5-9F3A45BA98AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E56176-3BBC-8645-BA4C-0420D94797E1}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
added hybrid changes to sitePreparationCost
</commit_message>
<xml_diff>
--- a/project_input_template/project_list.xlsx
+++ b/project_input_template/project_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/banderso2/Documents/PublicLandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F30DFB-9941-FE4E-AF46-C6635148FE3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36109B05-90FB-9C41-84F3-862C6D2B0008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Project list" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
     <t>Distance to interconnect [mi]</t>
   </si>
   <si>
-    <t>manual</t>
+    <t>auto</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="A1:AT4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU11" sqref="AU11"/>
+      <selection activeCell="AU40" sqref="AU40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added layout_length method to module parent class CostModule. It calculates the collection system length in manual mode, which is also equal to the base road length and is used in erection for crane travel distances. XlsxReader now reads in turbine spacings for auto mode, and the collection_layout input sheet for manual mode.
</commit_message>
<xml_diff>
--- a/project_input_template/project_list.xlsx
+++ b/project_input_template/project_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/banderso2/Documents/PublicLandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36109B05-90FB-9C41-84F3-862C6D2B0008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B978233-2A48-5848-91DB-06341F3F8BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
@@ -192,7 +192,7 @@
     <t>Distance to interconnect [mi]</t>
   </si>
   <si>
-    <t>auto</t>
+    <t>manual</t>
   </si>
 </sst>
 </file>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
   <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU40" sqref="AU40"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT13" sqref="AT13:AT14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
populate input template folder with data this contains all scenarios we will be testing DW integration into public LandBOSSE with . This expected validation data is results obtained using public data (with public component data). This commit should therefore pass in Travis CI
</commit_message>
<xml_diff>
--- a/project_input_template/project_list.xlsx
+++ b/project_input_template/project_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/landbosse-issue-103-validation-fails-2020-2-3-9-17-18/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF168283-26FA-1744-B3AC-D28650517811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EDA2F2-F0F9-0447-9687-EF2A86D30283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14360" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>Project ID</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Site prep area for Distributed wind (m2)</t>
   </si>
   <si>
-    <t>ge15_dist_01</t>
-  </si>
-  <si>
     <t>Override total management cost for distributed (0 does not override)</t>
   </si>
   <si>
@@ -182,7 +179,28 @@
     <t>Crane breakdown fraction</t>
   </si>
   <si>
-    <t>ge15_dist_project_data_public</t>
+    <t>clipper_25_public</t>
+  </si>
+  <si>
+    <t>ge15_public</t>
+  </si>
+  <si>
+    <t>iea36_85_project_data</t>
+  </si>
+  <si>
+    <t>iea36_120_project_data</t>
+  </si>
+  <si>
+    <t>foundation_validation_ge15</t>
+  </si>
+  <si>
+    <t>foundation_validation_clipper25</t>
+  </si>
+  <si>
+    <t>foundation_validation_iea36_85</t>
+  </si>
+  <si>
+    <t>foundation_validation_iea36_120</t>
   </si>
 </sst>
 </file>
@@ -221,18 +239,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -244,26 +256,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,120 +586,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:AT8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="3" width="28.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" customWidth="1"/>
-    <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="18" max="18" width="27.1640625" customWidth="1"/>
-    <col min="19" max="19" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="46" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.5" customWidth="1"/>
-    <col min="22" max="22" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20" customWidth="1"/>
-    <col min="27" max="27" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="28.1640625" customWidth="1"/>
-    <col min="30" max="30" width="25.5" customWidth="1"/>
-    <col min="31" max="31" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.6640625" customWidth="1"/>
-    <col min="33" max="33" width="23" customWidth="1"/>
-    <col min="34" max="34" width="27.5" customWidth="1"/>
-    <col min="35" max="35" width="22.1640625" customWidth="1"/>
-    <col min="36" max="36" width="24.6640625" customWidth="1"/>
-    <col min="37" max="37" width="26.6640625" customWidth="1"/>
-    <col min="38" max="38" width="55" style="7" customWidth="1"/>
-    <col min="39" max="39" width="32" customWidth="1"/>
-    <col min="40" max="40" width="27.1640625" customWidth="1"/>
-    <col min="41" max="41" width="22.6640625" customWidth="1"/>
-    <col min="42" max="42" width="34" customWidth="1"/>
-    <col min="43" max="43" width="24.6640625" customWidth="1"/>
-    <col min="44" max="44" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="28.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18" style="1" customWidth="1"/>
+    <col min="18" max="18" width="27.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="52.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.5" style="1" customWidth="1"/>
+    <col min="22" max="22" width="39.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.1640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="25.5" style="1" customWidth="1"/>
+    <col min="31" max="31" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="39.6640625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="23" style="1" customWidth="1"/>
+    <col min="34" max="34" width="27.5" style="1" customWidth="1"/>
+    <col min="35" max="35" width="22.1640625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="24.6640625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="26.6640625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="60.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="32" style="1" customWidth="1"/>
+    <col min="40" max="40" width="27.1640625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="22.6640625" style="1" customWidth="1"/>
+    <col min="42" max="42" width="34" style="1" customWidth="1"/>
+    <col min="43" max="43" width="24.6640625" style="1" customWidth="1"/>
+    <col min="44" max="44" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
       <c r="U1" t="s">
@@ -697,219 +709,647 @@
       <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AM1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AS1" t="s">
         <v>46</v>
       </c>
-      <c r="AS1" s="9" t="s">
+      <c r="AT1" t="s">
         <v>47</v>
-      </c>
-      <c r="AT1" s="10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
         <v>1.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>80</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>77</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>10</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
+      <c r="I2" s="1">
+        <v>100</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="1">
         <v>1.5</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="1">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>0.2</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>2.36</v>
       </c>
       <c r="O2" s="3">
         <v>589000</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <v>191521</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
         <v>59.5</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="1">
         <v>60</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>50</v>
+      </c>
+      <c r="U2" s="1">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1">
+        <v>15</v>
+      </c>
+      <c r="W2" s="2">
+        <v>5</v>
+      </c>
+      <c r="X2" s="2">
+        <v>130</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>10</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AQ2" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="2">
         <v>1</v>
       </c>
-      <c r="U2">
+      <c r="AT2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>80</v>
+      </c>
+      <c r="F3" s="1">
+        <v>96</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
         <v>10</v>
       </c>
-      <c r="V2">
+      <c r="I3" s="1">
+        <v>60</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>8</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>2.44</v>
+      </c>
+      <c r="O3" s="3">
+        <v>1009000</v>
+      </c>
+      <c r="P3" s="1">
+        <v>191521</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>59.5</v>
+      </c>
+      <c r="R3" s="1">
+        <v>60</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>50</v>
+      </c>
+      <c r="U3" s="1">
+        <v>10</v>
+      </c>
+      <c r="V3" s="1">
         <v>15</v>
       </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
+      <c r="W3" s="2">
+        <v>5</v>
+      </c>
+      <c r="X3" s="2">
+        <v>130</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>10</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AQ3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AR3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>85</v>
+      </c>
+      <c r="F4" s="1">
+        <v>130</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L4" s="1">
+        <v>6</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N4" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1261000</v>
+      </c>
+      <c r="P4" s="1">
+        <v>191521</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>52.5</v>
+      </c>
+      <c r="R4" s="1">
+        <v>60</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>50</v>
+      </c>
+      <c r="U4" s="1">
+        <v>10</v>
+      </c>
+      <c r="V4" s="1">
         <v>15</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="W4" s="2">
+        <v>5</v>
+      </c>
+      <c r="X4" s="2">
+        <v>130</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="5">
-        <v>500</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="4">
+      <c r="AF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>10</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AN4" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AO4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AQ4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AR4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="2">
         <v>1</v>
       </c>
-      <c r="AC2">
+      <c r="AT4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>120</v>
+      </c>
+      <c r="F5" s="1">
+        <v>130</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1">
+        <v>28</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>6</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N5" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1780000</v>
+      </c>
+      <c r="P5" s="1">
+        <v>191521</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>52.5</v>
+      </c>
+      <c r="R5" s="1">
+        <v>60</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>50</v>
+      </c>
+      <c r="U5" s="1">
+        <v>10</v>
+      </c>
+      <c r="V5" s="1">
+        <v>15</v>
+      </c>
+      <c r="W5" s="2">
+        <v>5</v>
+      </c>
+      <c r="X5" s="2">
+        <v>130</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AC5" s="2">
         <v>20</v>
       </c>
-      <c r="AD2">
+      <c r="AD5" s="2">
         <v>8</v>
       </c>
-      <c r="AE2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF2" s="5">
-        <v>4500</v>
-      </c>
-      <c r="AG2">
+      <c r="AE5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="2">
         <v>12.2</v>
       </c>
-      <c r="AH2">
-        <v>4</v>
-      </c>
-      <c r="AI2">
+      <c r="AH5" s="2">
+        <v>10</v>
+      </c>
+      <c r="AI5" s="2">
         <v>2</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ5" s="2">
         <v>1.4</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AK5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AL2" s="7">
-        <f>231750+1287500</f>
-        <v>1519250</v>
-      </c>
-      <c r="AM2">
+      <c r="AL5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="2">
         <v>0.03</v>
       </c>
-      <c r="AN2">
+      <c r="AN5" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
+      <c r="AO5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="2">
         <v>0.05</v>
       </c>
-      <c r="AQ2">
+      <c r="AQ5" s="2">
         <v>0.05</v>
       </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
-      <c r="AS2">
+      <c r="AR5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="2">
         <v>1</v>
       </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
+      <c r="AT5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A6"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="Z8" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Remove V47 scenario from validation portfolio. Since this turbine validation and NW 100 is still work in progress, under the DW development task for Q3 and Q4 of FY20
</commit_message>
<xml_diff>
--- a/project_input_template/project_list.xlsx
+++ b/project_input_template/project_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EDA2F2-F0F9-0447-9687-EF2A86D30283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E92F8D9-467E-9C45-ADA3-02D8FB7A067A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14360" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
@@ -589,7 +589,7 @@
   <dimension ref="A1:AT8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Extend management module to DW
</commit_message>
<xml_diff>
--- a/project_input_template/project_list.xlsx
+++ b/project_input_template/project_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F60EF5-3087-5342-A1F5-4C2E4FD69DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80C59B5-A3C6-2443-850B-BC4578DD3D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14360" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
   <dimension ref="A1:AT11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="AL17" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
couple input file value changes
</commit_message>
<xml_diff>
--- a/project_input_template/project_list.xlsx
+++ b/project_input_template/project_list.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/banderso2/Documents/PublicLandBOSSE/project_input_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/banderso2/Documents/BOS/PublicLandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B978233-2A48-5848-91DB-06341F3F8BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A94826-9D0A-7844-9665-E3FE269F3C1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Project list" sheetId="1" r:id="rId1"/>
     <sheet name="Parametric list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Project ID</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Foundation depth m</t>
   </si>
   <si>
-    <t>foundation_validation_ge15</t>
-  </si>
-  <si>
     <t>Rated Thrust (N)</t>
   </si>
   <si>
@@ -177,12 +174,6 @@
     <t>Site prep area for Distributed wind (m2)</t>
   </si>
   <si>
-    <t>private_foundation_validation_ge15</t>
-  </si>
-  <si>
-    <t>public_foundation_validation_ge15</t>
-  </si>
-  <si>
     <t>project_data_defaults</t>
   </si>
   <si>
@@ -193,6 +184,9 @@
   </si>
   <si>
     <t>manual</t>
+  </si>
+  <si>
+    <t>auto</t>
   </si>
 </sst>
 </file>
@@ -202,7 +196,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,6 +214,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -577,13 +577,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
   <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT13" sqref="AT13:AT14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="28.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -627,6 +627,7 @@
     <col min="43" max="43" width="60.33203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
@@ -634,10 +635,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -652,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -673,108 +674,108 @@
         <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="AJ1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="AO1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AR1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AS1" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="AT1" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
       </c>
       <c r="C2" s="1">
         <v>9</v>
@@ -843,7 +844,7 @@
         <v>130</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Z2" s="4">
         <v>5000</v>
@@ -873,7 +874,7 @@
         <v>1.4</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ2" s="4">
         <v>0.03</v>
@@ -900,21 +901,21 @@
         <v>0</v>
       </c>
       <c r="AR2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AS2" s="7">
         <v>0</v>
       </c>
       <c r="AT2" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>48</v>
+      <c r="A3" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>9</v>
@@ -983,7 +984,7 @@
         <v>130</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Z3" s="10">
         <v>5000</v>
@@ -1013,7 +1014,7 @@
         <v>1.4</v>
       </c>
       <c r="AI3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ3" s="10">
         <v>0.03</v>
@@ -1040,19 +1041,20 @@
         <v>0</v>
       </c>
       <c r="AR3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AS3">
         <v>0</v>
       </c>
       <c r="AT3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="O4" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>